<commit_message>
fix some small bugs
</commit_message>
<xml_diff>
--- a/pooling_problem_data/map_var_name_index_2022-06-14.xlsx
+++ b/pooling_problem_data/map_var_name_index_2022-06-14.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>pooling_problem</t>
   </si>
@@ -33,106 +33,127 @@
     <t>stoch_pooling_problem</t>
   </si>
   <si>
+    <t>second-stage</t>
+  </si>
+  <si>
+    <t>variables</t>
+  </si>
+  <si>
+    <t>flow: x[Arc("s1", "p1")]</t>
+  </si>
+  <si>
+    <t>y[1]</t>
+  </si>
+  <si>
+    <t>flow: x[Arc("s2", "p1")]</t>
+  </si>
+  <si>
+    <t>y[2]</t>
+  </si>
+  <si>
+    <t>flow: x[Arc("s3", "t1")]</t>
+  </si>
+  <si>
+    <t>y[3]</t>
+  </si>
+  <si>
+    <t>flow: x[Arc("s3", "t2")]</t>
+  </si>
+  <si>
+    <t>y[4]</t>
+  </si>
+  <si>
+    <t>flow: x[Arc("p1", "t1")]</t>
+  </si>
+  <si>
+    <t>y[5]</t>
+  </si>
+  <si>
+    <t>flow: x[Arc("p1", "t2")]</t>
+  </si>
+  <si>
+    <t>y[6]</t>
+  </si>
+  <si>
+    <t>q[s1]</t>
+  </si>
+  <si>
+    <t>y[7]</t>
+  </si>
+  <si>
+    <t>q[s2]</t>
+  </si>
+  <si>
+    <t>y[8]</t>
+  </si>
+  <si>
+    <t>q[s3]</t>
+  </si>
+  <si>
+    <t>y[9]</t>
+  </si>
+  <si>
+    <t>q[p1]</t>
+  </si>
+  <si>
+    <t>y[10]</t>
+  </si>
+  <si>
+    <t>q[t1]</t>
+  </si>
+  <si>
+    <t>y[11]</t>
+  </si>
+  <si>
+    <t>q[t2]</t>
+  </si>
+  <si>
+    <t>y[12]</t>
+  </si>
+  <si>
     <t>first-stage</t>
   </si>
   <si>
-    <t>variables</t>
-  </si>
-  <si>
-    <t>x[Arc("s1", "p1")]</t>
-  </si>
-  <si>
-    <t>y[1]</t>
-  </si>
-  <si>
-    <t>x[Arc("s2", "p1")]</t>
-  </si>
-  <si>
-    <t>y[2]</t>
-  </si>
-  <si>
-    <t>x[Arc("s3", "t1")]</t>
-  </si>
-  <si>
-    <t>y[3]</t>
-  </si>
-  <si>
-    <t>x[Arc("s3", "t2")]</t>
-  </si>
-  <si>
-    <t>y[4]</t>
-  </si>
-  <si>
-    <t>x[Arc("p1", "t1")]</t>
-  </si>
-  <si>
-    <t>y[5]</t>
-  </si>
-  <si>
-    <t>x[Arc("p1", "t2")]</t>
-  </si>
-  <si>
-    <t>y[6]</t>
-  </si>
-  <si>
-    <t>q[s1]</t>
-  </si>
-  <si>
-    <t>y[7]</t>
-  </si>
-  <si>
-    <t>q[s2]</t>
-  </si>
-  <si>
-    <t>y[8]</t>
-  </si>
-  <si>
-    <t>q[s3]</t>
-  </si>
-  <si>
-    <t>y[9]</t>
-  </si>
-  <si>
-    <t>q[p1]</t>
-  </si>
-  <si>
-    <t>y[10]</t>
-  </si>
-  <si>
-    <t>q[t1]</t>
-  </si>
-  <si>
-    <t>y[11]</t>
-  </si>
-  <si>
-    <t>q[t2]</t>
-  </si>
-  <si>
-    <t>y[12]</t>
-  </si>
-  <si>
-    <t>second-stage</t>
+    <t>binary variables</t>
+  </si>
+  <si>
+    <t>decision on: x[Arc("s1", "p1")]</t>
   </si>
   <si>
     <t>x[1]</t>
   </si>
   <si>
+    <t>decision on: x[Arc("s2", "p1")]</t>
+  </si>
+  <si>
     <t>x[2]</t>
   </si>
   <si>
+    <t>decision on: x[Arc("s3", "t1")]</t>
+  </si>
+  <si>
     <t>x[3]</t>
   </si>
   <si>
+    <t>decision on: x[Arc("s3", "t2")]</t>
+  </si>
+  <si>
     <t>x[4]</t>
   </si>
   <si>
+    <t>decision on: x[Arc("p1", "t1")]</t>
+  </si>
+  <si>
     <t>x[5]</t>
   </si>
   <si>
+    <t>decision on: x[Arc("p1", "t2")]</t>
+  </si>
+  <si>
     <t>x[6]</t>
   </si>
   <si>
-    <t>p1</t>
+    <t>decision on: p1</t>
   </si>
   <si>
     <t>x[7]</t>
@@ -610,63 +631,63 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>